<commit_message>
Updated file tracker with completed linked list problems
</commit_message>
<xml_diff>
--- a/ProgressTracker.xlsx
+++ b/ProgressTracker.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Murali/Desktop/Leetcode Completed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Murali/Desktop/LeetcodeCompleted/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Linkedin Problem List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Linked Lists</t>
   </si>
@@ -72,13 +72,28 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>Github Status</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/intersection-of-two-linked-lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle-ii/</t>
+  </si>
+  <si>
+    <t>Need to improve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,14 +104,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,18 +138,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,93 +422,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="151.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>